<commit_message>
until error page in toseesaderat
</commit_message>
<xml_diff>
--- a/Asgari_Tasks/Agari_Programing_Tasks.xlsx
+++ b/Asgari_Tasks/Agari_Programing_Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programming_Practice\Asgari_Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6390C33C-E8A8-4246-9C2B-3DB6A10D6A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CF8B36-F2AF-4F60-A687-78625A67C0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5A913C81-908C-4EEF-8420-5EA9E3549327}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>ردیف</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>1403/08/07</t>
+  </si>
+  <si>
+    <t>لیست تمام شعب کل بانک های کشور</t>
+  </si>
+  <si>
+    <t>تمام بانک های کشور مشخص شود و ابتدا یک لیست درست شود که از چه طریقی می توان به لیست شعب رسید مثلا خودشون فرم اکسل دارن یا نه یه جدوله که با پایتون میشه خوندش یا نه هچ شعبی نداره یا پیدا نمیشه و بعد ایچاد یک اکسل بزرگ اطلاعات به ترتیب باشه برای همه بانک ها</t>
+  </si>
+  <si>
+    <t>بانک ملت</t>
+  </si>
+  <si>
+    <t>1403/08/10</t>
   </si>
 </sst>
 </file>
@@ -106,19 +118,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,16 +449,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33CED5E-B54D-4998-B68C-2DDCAC85F1B4}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="24.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="49.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" style="1" customWidth="1"/>
     <col min="5" max="6" width="8.88671875" style="1"/>
@@ -474,13 +489,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -498,9 +513,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
@@ -516,9 +531,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -533,11 +548,50 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>18.5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1">
+        <f>F5-E5</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bank data is stopped and calendar is started
</commit_message>
<xml_diff>
--- a/Asgari_Tasks/Agari_Programing_Tasks.xlsx
+++ b/Asgari_Tasks/Agari_Programing_Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programming_Practice\Asgari_Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CF8B36-F2AF-4F60-A687-78625A67C0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E5AA8E-B663-47D4-9A41-2E8CA2BA9253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5A913C81-908C-4EEF-8420-5EA9E3549327}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>ردیف</t>
   </si>
@@ -73,6 +73,36 @@
   </si>
   <si>
     <t>1403/08/10</t>
+  </si>
+  <si>
+    <t>رسیدن به مرحله استخراج اکسل هر کدوم از بانک ها</t>
+  </si>
+  <si>
+    <t>متاسفانه تا این مرحله یادم رفت ساعت کاری رو درج کنم و این یک زمان حدودی انجام کار است که در این تاریخ زده می شود</t>
+  </si>
+  <si>
+    <t>1403/09/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ساخت اکسل کامل </t>
+  </si>
+  <si>
+    <t>در این مرحله یک اکسل بزرگ از اطلاعات همه ی بانک ها ساخته می شود</t>
+  </si>
+  <si>
+    <t>در انجام این مرحله یک سری اکسل امکان خوانده شدن نداشتن که این مدت به رفع این مشکل گذشت</t>
+  </si>
+  <si>
+    <t>1403/09/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ساخت تقویم </t>
+  </si>
+  <si>
+    <t>در این مرحله دیتای سال ۱۴۰۳ تا حد شکل گیری تقویم جمع َآوری شد و تقویم ساخته شد ولی اطلاعات ماه قمری جهت تعیطلات اشتباه است</t>
+  </si>
+  <si>
+    <t>1403/09/14</t>
   </si>
 </sst>
 </file>
@@ -118,13 +148,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -449,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33CED5E-B54D-4998-B68C-2DDCAC85F1B4}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,13 +522,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -508,14 +541,14 @@
         <v>4.5</v>
       </c>
       <c r="G2" s="1">
-        <f>F2-E2</f>
+        <f t="shared" ref="G2:G11" si="0">F2-E2</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
@@ -526,14 +559,14 @@
         <v>20.5</v>
       </c>
       <c r="G3" s="1">
-        <f>F3-E3</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
@@ -544,15 +577,15 @@
         <v>2.5</v>
       </c>
       <c r="G4" s="1">
-        <f>F4-E4</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -568,13 +601,13 @@
         <v>21</v>
       </c>
       <c r="G5" s="1">
-        <f>F5-E5</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
@@ -584,9 +617,129 @@
       <c r="E6" s="1">
         <v>1.5</v>
       </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A2:A4"/>

</xml_diff>

<commit_message>
calendar is almost done
</commit_message>
<xml_diff>
--- a/Asgari_Tasks/Agari_Programing_Tasks.xlsx
+++ b/Asgari_Tasks/Agari_Programing_Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programming_Practice\Asgari_Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E5AA8E-B663-47D4-9A41-2E8CA2BA9253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61AEDF0-FC34-4C42-9150-2AF1EF7CC847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5A913C81-908C-4EEF-8420-5EA9E3549327}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>ردیف</t>
   </si>
@@ -103,6 +103,24 @@
   </si>
   <si>
     <t>1403/09/14</t>
+  </si>
+  <si>
+    <t>بهتر کردن شکل ظاهری تقویم و تبدیل table به div</t>
+  </si>
+  <si>
+    <t>1403/09/15</t>
+  </si>
+  <si>
+    <t>اضافه کردن دو سال دیگر و تغییر عملکرد بر اساس آن ها و بهبود ظاهر</t>
+  </si>
+  <si>
+    <t>1403/09/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اضافه کردن فونت فارسی مناسب </t>
+  </si>
+  <si>
+    <t>1403/09/18</t>
   </si>
 </sst>
 </file>
@@ -148,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -167,6 +185,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33CED5E-B54D-4998-B68C-2DDCAC85F1B4}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +562,7 @@
         <v>4.5</v>
       </c>
       <c r="G2" s="1">
-        <f t="shared" ref="G2:G11" si="0">F2-E2</f>
+        <f t="shared" ref="G2:G14" si="0">F2-E2</f>
         <v>1</v>
       </c>
     </row>
@@ -712,10 +733,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="7">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -735,11 +756,71 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1">
+        <v>16</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="5"/>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B11:B14"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A2:A4"/>

</xml_diff>

<commit_message>
everything stops and asp.net starts
</commit_message>
<xml_diff>
--- a/Asgari_Tasks/Agari_Programing_Tasks.xlsx
+++ b/Asgari_Tasks/Agari_Programing_Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programming_Practice\Asgari_Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61AEDF0-FC34-4C42-9150-2AF1EF7CC847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10CA419-9A9F-47D0-9F21-D38F43F14831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5A913C81-908C-4EEF-8420-5EA9E3549327}"/>
+    <workbookView xWindow="5760" yWindow="2952" windowWidth="17280" windowHeight="8880" xr2:uid="{5A913C81-908C-4EEF-8420-5EA9E3549327}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -185,9 +185,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33CED5E-B54D-4998-B68C-2DDCAC85F1B4}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,7 +730,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -757,7 +754,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
         <v>26</v>
@@ -777,7 +774,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
         <v>28</v>
@@ -797,6 +794,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
         <v>30</v>
@@ -816,7 +814,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
@@ -826,6 +824,7 @@
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>